<commit_message>
Versión 2.0 - Actualización al 1 de Agosto de 2021
</commit_message>
<xml_diff>
--- a/Resources/data/ISA - Retorno Países OCDE y AL_Isa actualización julio.xlsx
+++ b/Resources/data/ISA - Retorno Países OCDE y AL_Isa actualización julio.xlsx
@@ -809,6 +809,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>El 1 de febrero, el Departamento de Educación acordó reabrir las escuelas especiales con un 50% de capacidad el jueves 11 de febrero y las clases especiales en las escuelas ordinarias el lunes 22 de febrero. [82] [83] [84] El jueves 11 de febrero, hasta 4.000 niños con necesidades educativas adicionales regresaron a la educación presencial cuando las escuelas especiales de todo el país reabrieron sus puertas, según los planes acordados entre el Departamento de Educación y los sindicatos de maestros y SNA. . [85] [86] [87]</t>
     </r>
     <r>
@@ -918,6 +926,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">Se inició con alumnos de preescolar y de los primeros cuatro cursos de primaria. 20% del alumnado, el 80% restante (1,9 millones de estudiantes) seguirá con clases virtuales, y su vuelta se hará en varias fases para evitar un nuevo pico de infecciones.
 Primera fase, preescolar y hasta los 10 años, en las llamadas zonas verdes, con bajo índice de morbilidad, o en las que más de un 70% de la población por encima de los 50 años ha sido vacunada.
 La segunda fase, a partir del 23 de febrero, contempla la vuelta a las aulas a partir de los 10 a los 18 años en ciudades con bajo índice de contagios o con más del 70% de vacunación.
@@ -985,6 +999,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">Es el segundo intento de reincoporación, la primera fue en agosto 2020.
 El Ministerio de Educación había dado instrucciones de seguridad: los cubrebocas debían ser usados por los estudiantes a partir de cuarto grado, las ventanas tenían que estar abiertas, debían lavarse las manos con frecuencia y los estudiantes tenían que mantener una distancia de dos metros siempre que fuera posible.
 Para la reincorporación a clases en el año 2021 se utilizará el modelo "10-4"desarrollado por los científicos Uri Alon y Ron Milo, y se basa en el período de latencia del virus, es decir, el lapso que transcurre entre que una persona se contagia y pasa a ser contagiosa para los demás. Ese tiempo se calcula en tres días y de ahí surge el modelo: 4 días en la escuela (de lunes a jueves) y 10 días de confinamiento, lo que da oportunidad para ingresar a un nuevo grupo de alumnos y se reduzca la posibilidad de segregación de la enfermedad.
@@ -1137,14 +1158,14 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
     <numFmt numFmtId="176" formatCode="dd\-mmm"/>
-    <numFmt numFmtId="177" formatCode="mmm\-yy"/>
-    <numFmt numFmtId="178" formatCode="dd\-mmm\-yy"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="dd\-mmm\-yy"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="mmm\-yy"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1170,13 +1191,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1213,11 +1227,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color theme="0"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1229,75 +1242,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1312,38 +1257,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1359,9 +1273,93 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1413,7 +1411,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1425,25 +1531,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1455,19 +1549,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1479,67 +1567,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1551,31 +1579,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1587,13 +1591,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1633,26 +1631,33 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1674,24 +1679,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1715,155 +1707,161 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1872,9 +1870,9 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1897,23 +1895,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1922,13 +1920,13 @@
     <xf numFmtId="58" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="48" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="48" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="48" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="48" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1940,31 +1938,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="48" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="48" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="48" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="48" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1973,16 +1965,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="48" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="48" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2064,16 +2056,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>770255</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2503805</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>704850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>3834130</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>512445</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>923925</xdr:rowOff>
+      <xdr:rowOff>1590675</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2090,7 +2082,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="770255" y="1171575"/>
+          <a:off x="9792970" y="1838325"/>
           <a:ext cx="26676350" cy="4867275"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2619,48 +2611,48 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="39">
+      <c r="B4" s="37">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="39">
+      <c r="B5" s="37">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="39">
+      <c r="B6" s="37">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="39">
+      <c r="B7" s="37">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="39"/>
+      <c r="B8" s="37"/>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="39">
+      <c r="B9" s="37">
         <v>30</v>
       </c>
     </row>
@@ -2755,47 +2747,47 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" s="32" customFormat="1" ht="45" hidden="1" customHeight="1" spans="1:14">
-      <c r="A3" s="33" t="s">
+    <row r="3" s="30" customFormat="1" ht="45" hidden="1" customHeight="1" spans="1:14">
+      <c r="A3" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="35">
+      <c r="E3" s="33">
         <v>44287</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="36" t="s">
+      <c r="G3" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="33" t="s">
+      <c r="I3" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="33" t="s">
+      <c r="J3" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="33" t="s">
+      <c r="K3" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="33" t="s">
+      <c r="L3" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="33" t="s">
+      <c r="M3" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="N3" s="37" t="s">
+      <c r="N3" s="35" t="s">
         <v>29</v>
       </c>
     </row>
@@ -3443,7 +3435,7 @@
       <c r="M21" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="N21" s="30" t="s">
+      <c r="N21" s="25" t="s">
         <v>103</v>
       </c>
     </row>
@@ -3551,7 +3543,7 @@
       <c r="M24" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="N24" s="28" t="s">
+      <c r="N24" s="27" t="s">
         <v>115</v>
       </c>
     </row>
@@ -3895,7 +3887,7 @@
       <c r="M35" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="N35" s="28" t="s">
+      <c r="N35" s="27" t="s">
         <v>152</v>
       </c>
     </row>
@@ -4076,7 +4068,7 @@
       <c r="M41" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="N41" s="29" t="s">
+      <c r="N41" s="28" t="s">
         <v>169</v>
       </c>
     </row>
@@ -4164,7 +4156,7 @@
       <c r="M43" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="N43" s="30" t="s">
+      <c r="N43" s="25" t="s">
         <v>180</v>
       </c>
     </row>
@@ -4208,7 +4200,7 @@
       <c r="M44" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="N44" s="30" t="s">
+      <c r="N44" s="25" t="s">
         <v>185</v>
       </c>
     </row>
@@ -4508,7 +4500,7 @@
       <c r="M53" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="N53" s="31" t="s">
+      <c r="N53" s="29" t="s">
         <v>218</v>
       </c>
     </row>
@@ -4627,9 +4619,9 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -5540,7 +5532,7 @@
       <c r="M21" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="N21" s="28" t="s">
+      <c r="N21" s="27" t="s">
         <v>152</v>
       </c>
     </row>
@@ -5629,7 +5621,7 @@
       <c r="M23" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="N23" s="29" t="s">
+      <c r="N23" s="28" t="s">
         <v>169</v>
       </c>
     </row>
@@ -5717,7 +5709,7 @@
       <c r="M25" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="N25" s="30" t="s">
+      <c r="N25" s="25" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5761,7 +5753,7 @@
       <c r="M26" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="N26" s="30" t="s">
+      <c r="N26" s="25" t="s">
         <v>185</v>
       </c>
     </row>
@@ -5981,7 +5973,7 @@
       <c r="M31" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="N31" s="31" t="s">
+      <c r="N31" s="29" t="s">
         <v>218</v>
       </c>
     </row>

</xml_diff>